<commit_message>
Change note on units in csv files
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
+++ b/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\BFoCPAbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\BFoCPAbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52A2814-F7F6-4B4A-87A1-E70FE98E2B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C255099-C710-46E8-8FB3-8FE1851643E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -509,9 +509,6 @@
     <t>Figure 5</t>
   </si>
   <si>
-    <t>Unit: g CO2 captured</t>
-  </si>
-  <si>
     <t>*ethanol mapped to the chemicals industry, ammonia not counted because we assume this industry is decarbonized through the hydrogen PTC</t>
   </si>
   <si>
@@ -1383,6 +1380,9 @@
   </si>
   <si>
     <t>BFoCPAbS BAU Fraction of CCS Potential Achieved by Industry</t>
+  </si>
+  <si>
+    <t>Unit: Dmnl</t>
   </si>
 </sst>
 </file>
@@ -2051,7 +2051,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2059,7 +2059,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2092,7 +2092,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2107,22 +2107,22 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2165,12 +2165,12 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2189,7 +2189,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3566,7 +3566,7 @@
         <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3583,7 +3583,7 @@
         <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3701,7 +3701,7 @@
         <v>194</v>
       </c>
       <c r="E53" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3726,12 +3726,12 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3">
         <v>2021</v>
@@ -3826,7 +3826,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" s="38">
         <v>8000000000000</v>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" s="38">
         <v>2200000000000</v>
@@ -4016,7 +4016,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B6" s="38">
         <v>33800000000000</v>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B7" s="38">
         <v>0</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8" s="38">
         <v>0</v>
@@ -4301,7 +4301,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="38">
         <v>0</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10" s="38">
         <v>0</v>
@@ -4491,7 +4491,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" s="38">
         <v>0</v>
@@ -4586,7 +4586,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="38">
         <v>2300000000000</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B13" s="38">
         <v>49700000000000</v>
@@ -4776,7 +4776,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="38">
         <v>0</v>
@@ -4871,7 +4871,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4966,7 +4966,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B16" s="38">
         <v>63800000000000</v>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B17" s="38">
         <v>36800000000000</v>
@@ -5156,7 +5156,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18" s="38">
         <v>4400000000000</v>
@@ -5251,7 +5251,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B19" s="38">
         <v>0</v>
@@ -5346,7 +5346,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B20" s="38">
         <v>1007000000</v>
@@ -5441,7 +5441,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B21" s="38">
         <v>0</v>
@@ -5536,7 +5536,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B22" s="38">
         <v>0</v>
@@ -5631,7 +5631,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B23" s="38">
         <v>0</v>
@@ -5726,7 +5726,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B24" s="38">
         <v>0</v>
@@ -5821,7 +5821,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B25" s="38">
         <v>0</v>
@@ -5916,7 +5916,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B26" s="38">
         <v>27500000000000</v>
@@ -6011,7 +6011,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -6106,7 +6106,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B28" s="38">
         <v>0</v>
@@ -6233,7 +6233,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B30">
         <v>2021</v>
@@ -6328,7 +6328,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B31" s="38">
         <v>0</v>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B32" s="38">
         <v>0</v>
@@ -6518,7 +6518,7 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B33" s="38">
         <v>0</v>
@@ -6613,7 +6613,7 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B34" s="38">
         <v>0</v>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B35" s="38">
         <v>0</v>
@@ -6803,7 +6803,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B36" s="38">
         <v>0</v>
@@ -6898,7 +6898,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B37" s="38">
         <v>0</v>
@@ -6993,7 +6993,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" s="38">
         <v>0</v>
@@ -7088,7 +7088,7 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -7183,7 +7183,7 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -7278,7 +7278,7 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -7373,7 +7373,7 @@
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -7468,7 +7468,7 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -7563,7 +7563,7 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -7658,7 +7658,7 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -7753,7 +7753,7 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -7848,7 +7848,7 @@
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -7943,7 +7943,7 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -8038,7 +8038,7 @@
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -8133,7 +8133,7 @@
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -8228,7 +8228,7 @@
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -8323,7 +8323,7 @@
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -8418,7 +8418,7 @@
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -8513,7 +8513,7 @@
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -8608,7 +8608,7 @@
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -8703,7 +8703,7 @@
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -8798,7 +8798,7 @@
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -8893,7 +8893,7 @@
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B58" s="38">
         <v>19502000000</v>
@@ -8988,7 +8988,7 @@
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B59" s="38">
         <v>2092490000000</v>
@@ -9083,7 +9083,7 @@
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B60" s="38">
         <v>11632100000000</v>
@@ -9178,7 +9178,7 @@
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B61" s="38">
         <v>106076000000</v>
@@ -9273,7 +9273,7 @@
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -9368,7 +9368,7 @@
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B63" s="38">
         <v>5190830000000</v>
@@ -9463,7 +9463,7 @@
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B64" s="38">
         <v>2272080000000</v>
@@ -9558,7 +9558,7 @@
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B65" s="38">
         <v>9334890000000</v>
@@ -9653,7 +9653,7 @@
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -9748,7 +9748,7 @@
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -9843,7 +9843,7 @@
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B68" s="38">
         <v>16366600000000</v>
@@ -9938,7 +9938,7 @@
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B69" s="38">
         <v>3431200000000</v>
@@ -10033,7 +10033,7 @@
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B70" s="38">
         <v>91263500000</v>
@@ -10128,7 +10128,7 @@
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -10223,7 +10223,7 @@
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -10318,7 +10318,7 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -10413,7 +10413,7 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -10508,7 +10508,7 @@
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -10603,7 +10603,7 @@
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -10698,7 +10698,7 @@
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B77" s="38">
         <v>331286000000</v>
@@ -10793,7 +10793,7 @@
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -10888,7 +10888,7 @@
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -10983,7 +10983,7 @@
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -11078,7 +11078,7 @@
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B81" s="38">
         <v>4960930000000</v>
@@ -11173,7 +11173,7 @@
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B82" s="38">
         <v>7932630000000</v>
@@ -11268,7 +11268,7 @@
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B83" s="38">
         <v>108060000000000</v>
@@ -11363,7 +11363,7 @@
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B84" s="38">
         <v>11110900000000</v>
@@ -11458,7 +11458,7 @@
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B85" s="38">
         <v>48585900000000</v>
@@ -11553,7 +11553,7 @@
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B86" s="38">
         <v>5537710000000</v>
@@ -11648,7 +11648,7 @@
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B87" s="38">
         <v>3097290000000</v>
@@ -11743,7 +11743,7 @@
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B88" s="38">
         <v>29767700000000</v>
@@ -11838,7 +11838,7 @@
     </row>
     <row r="89" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B89" s="38">
         <v>43963500000000</v>
@@ -11933,7 +11933,7 @@
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B90" s="38">
         <v>108608000000000</v>
@@ -12028,7 +12028,7 @@
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B91" s="38">
         <v>4303610000000</v>
@@ -12123,7 +12123,7 @@
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B92" s="38">
         <v>5723100000000</v>
@@ -12218,7 +12218,7 @@
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B93" s="38">
         <v>4350300000000</v>
@@ -12313,7 +12313,7 @@
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B94" s="38">
         <v>0</v>
@@ -12408,7 +12408,7 @@
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B95" s="38">
         <v>10152700000000</v>
@@ -12503,7 +12503,7 @@
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B96" s="38">
         <v>5876500000000</v>
@@ -12598,7 +12598,7 @@
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B97" s="38">
         <v>1637870000000</v>
@@ -12693,7 +12693,7 @@
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B98" s="38">
         <v>1650940000000</v>
@@ -12788,7 +12788,7 @@
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B99" s="38">
         <v>2892370000000</v>
@@ -12883,7 +12883,7 @@
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B100" s="38">
         <v>5139370000000</v>
@@ -12978,7 +12978,7 @@
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B101" s="38">
         <v>2909440000000</v>
@@ -13073,7 +13073,7 @@
     </row>
     <row r="102" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B102" s="38">
         <v>17295000000000</v>
@@ -13168,7 +13168,7 @@
     </row>
     <row r="103" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B103" s="38">
         <v>55637100000000</v>
@@ -13263,7 +13263,7 @@
     </row>
     <row r="104" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B104" s="38">
         <v>0</v>
@@ -13358,7 +13358,7 @@
     </row>
     <row r="105" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B105" s="38">
         <v>11695200000000</v>
@@ -13453,7 +13453,7 @@
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B106" s="38">
         <v>0</v>
@@ -13548,7 +13548,7 @@
     </row>
     <row r="107" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B107" s="38">
         <v>0</v>
@@ -13643,7 +13643,7 @@
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B108" s="38">
         <v>0</v>
@@ -13738,7 +13738,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -13833,7 +13833,7 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B110" s="38">
         <v>0</v>
@@ -13928,7 +13928,7 @@
     </row>
     <row r="111" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -14023,7 +14023,7 @@
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B112" s="38">
         <v>0</v>
@@ -14118,7 +14118,7 @@
     </row>
     <row r="113" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B113" s="38">
         <v>0</v>
@@ -14213,7 +14213,7 @@
     </row>
     <row r="114" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B114" s="38">
         <v>0</v>
@@ -14308,7 +14308,7 @@
     </row>
     <row r="115" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B115" s="38">
         <v>0</v>
@@ -14403,7 +14403,7 @@
     </row>
     <row r="116" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B116" s="38">
         <v>0</v>
@@ -14498,7 +14498,7 @@
     </row>
     <row r="117" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B117" s="38">
         <v>0</v>
@@ -14593,7 +14593,7 @@
     </row>
     <row r="118" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B118" s="38">
         <v>0</v>
@@ -14688,7 +14688,7 @@
     </row>
     <row r="119" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B119" s="38">
         <v>0</v>
@@ -14783,7 +14783,7 @@
     </row>
     <row r="120" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B120" s="38">
         <v>0</v>
@@ -14878,7 +14878,7 @@
     </row>
     <row r="121" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B121" s="38">
         <v>0</v>
@@ -14973,7 +14973,7 @@
     </row>
     <row r="122" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B122" s="38">
         <v>0</v>
@@ -15068,7 +15068,7 @@
     </row>
     <row r="123" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B123" s="38">
         <v>0</v>
@@ -15163,7 +15163,7 @@
     </row>
     <row r="124" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -15258,7 +15258,7 @@
     </row>
     <row r="125" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -15353,7 +15353,7 @@
     </row>
     <row r="126" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -15448,7 +15448,7 @@
     </row>
     <row r="127" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -15543,7 +15543,7 @@
     </row>
     <row r="128" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -15638,7 +15638,7 @@
     </row>
     <row r="129" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -15733,7 +15733,7 @@
     </row>
     <row r="130" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -15828,7 +15828,7 @@
     </row>
     <row r="131" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B131" s="38">
         <v>35940700000000</v>
@@ -15923,7 +15923,7 @@
     </row>
     <row r="132" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B132" s="38">
         <v>2761920000000</v>
@@ -16018,7 +16018,7 @@
     </row>
     <row r="133" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B133" s="38">
         <v>8379870000000</v>
@@ -16113,7 +16113,7 @@
     </row>
     <row r="134" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B134" s="38">
         <v>8506080000000</v>
@@ -16208,7 +16208,7 @@
     </row>
     <row r="135" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B135" s="38">
         <v>2368720000000</v>
@@ -16303,7 +16303,7 @@
     </row>
     <row r="136" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B136" s="38">
         <v>982499000000</v>
@@ -16398,7 +16398,7 @@
     </row>
     <row r="137" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B137" s="38">
         <v>612997000000</v>
@@ -16493,7 +16493,7 @@
     </row>
     <row r="138" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B138" s="38">
         <v>344397000000</v>
@@ -16588,7 +16588,7 @@
     </row>
     <row r="139" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -16683,7 +16683,7 @@
     </row>
     <row r="140" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B140" s="38">
         <v>85828500000</v>
@@ -16778,7 +16778,7 @@
     </row>
     <row r="141" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -16873,7 +16873,7 @@
     </row>
     <row r="142" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -16968,7 +16968,7 @@
     </row>
     <row r="143" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B143" s="38">
         <v>1625460000000</v>
@@ -17063,7 +17063,7 @@
     </row>
     <row r="144" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B144" s="38">
         <v>309260000000</v>
@@ -17158,7 +17158,7 @@
     </row>
     <row r="145" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B145" s="38">
         <v>922309000000</v>
@@ -17253,7 +17253,7 @@
     </row>
     <row r="146" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -17348,7 +17348,7 @@
     </row>
     <row r="147" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -17443,7 +17443,7 @@
     </row>
     <row r="148" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B148" s="38">
         <v>0</v>
@@ -17538,7 +17538,7 @@
     </row>
     <row r="149" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B149" s="38">
         <v>86011600000</v>
@@ -17633,7 +17633,7 @@
     </row>
     <row r="150" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B150" s="38">
         <v>163681000000</v>
@@ -17728,7 +17728,7 @@
     </row>
     <row r="151" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B151" s="38">
         <v>92660900000</v>
@@ -17823,7 +17823,7 @@
     </row>
     <row r="152" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B152" s="38">
         <v>3068450000000</v>
@@ -17918,7 +17918,7 @@
     </row>
     <row r="153" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B153" s="38">
         <v>0</v>
@@ -18013,7 +18013,7 @@
     </row>
     <row r="154" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B154" s="38">
         <v>0</v>
@@ -18108,7 +18108,7 @@
     </row>
     <row r="155" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B155" s="38">
         <v>44833300000000</v>
@@ -18203,7 +18203,7 @@
     </row>
     <row r="156" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B156" s="38">
         <v>0</v>
@@ -18298,7 +18298,7 @@
     </row>
     <row r="157" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -18393,7 +18393,7 @@
     </row>
     <row r="158" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -18488,7 +18488,7 @@
     </row>
     <row r="159" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -18583,7 +18583,7 @@
     </row>
     <row r="160" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B160" s="38">
         <v>0</v>
@@ -18678,7 +18678,7 @@
     </row>
     <row r="161" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B161" s="38">
         <v>0</v>
@@ -18773,7 +18773,7 @@
     </row>
     <row r="162" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B162" s="38">
         <v>0</v>
@@ -18868,7 +18868,7 @@
     </row>
     <row r="163" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B163" s="38">
         <v>0</v>
@@ -18963,7 +18963,7 @@
     </row>
     <row r="164" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B164" s="38">
         <v>0</v>
@@ -19058,7 +19058,7 @@
     </row>
     <row r="165" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B165" s="38">
         <v>0</v>
@@ -19153,7 +19153,7 @@
     </row>
     <row r="166" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B166" s="38">
         <v>0</v>
@@ -19248,7 +19248,7 @@
     </row>
     <row r="167" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B167" s="38">
         <v>0</v>
@@ -19343,7 +19343,7 @@
     </row>
     <row r="168" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B168" s="38">
         <v>0</v>
@@ -19438,7 +19438,7 @@
     </row>
     <row r="169" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -19533,7 +19533,7 @@
     </row>
     <row r="170" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -19628,7 +19628,7 @@
     </row>
     <row r="171" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -19723,7 +19723,7 @@
     </row>
     <row r="172" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B172" s="38">
         <v>0</v>
@@ -19818,7 +19818,7 @@
     </row>
     <row r="173" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B173" s="38">
         <v>0</v>
@@ -19913,7 +19913,7 @@
     </row>
     <row r="174" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B174" s="38">
         <v>0</v>
@@ -20008,7 +20008,7 @@
     </row>
     <row r="175" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B175" s="38">
         <v>0</v>
@@ -20103,7 +20103,7 @@
     </row>
     <row r="176" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B176" s="38">
         <v>0</v>
@@ -20198,7 +20198,7 @@
     </row>
     <row r="177" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B177" s="38">
         <v>0</v>
@@ -20293,7 +20293,7 @@
     </row>
     <row r="178" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B178" s="38">
         <v>0</v>
@@ -20388,7 +20388,7 @@
     </row>
     <row r="179" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B179" s="38">
         <v>0</v>
@@ -20483,7 +20483,7 @@
     </row>
     <row r="180" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B180" s="38">
         <v>0</v>
@@ -20578,7 +20578,7 @@
     </row>
     <row r="181" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -20673,7 +20673,7 @@
     </row>
     <row r="182" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -20768,7 +20768,7 @@
     </row>
     <row r="183" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B183" s="38">
         <v>0</v>
@@ -20863,7 +20863,7 @@
     </row>
     <row r="184" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -20958,7 +20958,7 @@
     </row>
     <row r="185" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -21053,7 +21053,7 @@
     </row>
     <row r="186" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -21148,7 +21148,7 @@
     </row>
     <row r="187" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -21243,7 +21243,7 @@
     </row>
     <row r="188" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -21338,7 +21338,7 @@
     </row>
     <row r="189" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B189" s="38">
         <v>132433000000000</v>
@@ -21433,7 +21433,7 @@
     </row>
     <row r="190" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -21528,7 +21528,7 @@
     </row>
     <row r="191" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -21623,7 +21623,7 @@
     </row>
     <row r="192" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -21718,7 +21718,7 @@
     </row>
     <row r="193" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -21813,7 +21813,7 @@
     </row>
     <row r="194" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -21908,7 +21908,7 @@
     </row>
     <row r="195" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -22003,7 +22003,7 @@
     </row>
     <row r="196" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B196" s="38">
         <v>0</v>
@@ -22098,7 +22098,7 @@
     </row>
     <row r="197" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -22193,7 +22193,7 @@
     </row>
     <row r="198" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -22288,7 +22288,7 @@
     </row>
     <row r="199" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -22383,7 +22383,7 @@
     </row>
     <row r="200" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -22478,7 +22478,7 @@
     </row>
     <row r="201" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -22573,7 +22573,7 @@
     </row>
     <row r="202" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -22668,7 +22668,7 @@
     </row>
     <row r="203" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -22763,7 +22763,7 @@
     </row>
     <row r="204" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -22858,7 +22858,7 @@
     </row>
     <row r="205" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -22953,7 +22953,7 @@
     </row>
     <row r="206" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B206" s="38">
         <v>16453000000</v>
@@ -23048,7 +23048,7 @@
     </row>
     <row r="207" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B207" s="38">
         <v>59246200000</v>
@@ -23143,7 +23143,7 @@
     </row>
     <row r="208" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B208" s="38">
         <v>322572000000</v>
@@ -23238,7 +23238,7 @@
     </row>
     <row r="209" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B209">
         <v>0</v>
@@ -23333,7 +23333,7 @@
     </row>
     <row r="210" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B210" s="38">
         <v>28550500000</v>
@@ -23428,7 +23428,7 @@
     </row>
     <row r="211" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B211" s="38">
         <v>14411100000</v>
@@ -23523,7 +23523,7 @@
     </row>
     <row r="212" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -23618,7 +23618,7 @@
     </row>
     <row r="213" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B213" s="38">
         <v>2067700000000</v>
@@ -23713,7 +23713,7 @@
     </row>
     <row r="214" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -23808,7 +23808,7 @@
     </row>
     <row r="215" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B215" s="38">
         <v>263361000000</v>
@@ -23903,7 +23903,7 @@
     </row>
     <row r="216" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B216" s="38">
         <v>8486300</v>
@@ -23998,7 +23998,7 @@
     </row>
     <row r="217" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B217">
         <v>0</v>
@@ -24093,7 +24093,7 @@
     </row>
     <row r="218" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -24188,7 +24188,7 @@
     </row>
     <row r="219" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -24283,7 +24283,7 @@
     </row>
     <row r="220" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B220" s="38">
         <v>12398800000</v>
@@ -24378,7 +24378,7 @@
     </row>
     <row r="221" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B221" s="38">
         <v>393749000</v>
@@ -24473,7 +24473,7 @@
     </row>
     <row r="222" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B222" s="38">
         <v>3679900</v>
@@ -24568,7 +24568,7 @@
     </row>
     <row r="223" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -24663,7 +24663,7 @@
     </row>
     <row r="224" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B224" s="38">
         <v>21628800</v>
@@ -24758,7 +24758,7 @@
     </row>
     <row r="225" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B225" s="38">
         <v>178015000000</v>
@@ -24853,7 +24853,7 @@
     </row>
     <row r="226" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B226" s="38">
         <v>100776000000</v>
@@ -24948,7 +24948,7 @@
     </row>
     <row r="227" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B227" s="38">
         <v>45007600000</v>
@@ -25043,7 +25043,7 @@
     </row>
     <row r="228" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -25138,7 +25138,7 @@
     </row>
     <row r="229" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -25233,7 +25233,7 @@
     </row>
     <row r="230" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -25328,7 +25328,7 @@
     </row>
     <row r="231" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B231" s="38">
         <v>5608430000000</v>
@@ -25423,7 +25423,7 @@
     </row>
     <row r="232" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -25518,7 +25518,7 @@
     </row>
     <row r="233" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -25613,7 +25613,7 @@
     </row>
     <row r="234" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -25708,7 +25708,7 @@
     </row>
     <row r="235" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B235" s="38">
         <v>257088000000</v>
@@ -25803,7 +25803,7 @@
     </row>
     <row r="236" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B236" s="38">
         <v>61737800000</v>
@@ -25898,7 +25898,7 @@
     </row>
     <row r="237" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B237" s="38">
         <v>96430100000</v>
@@ -25993,7 +25993,7 @@
     </row>
     <row r="238" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B238" s="38">
         <v>35762800000</v>
@@ -26088,7 +26088,7 @@
     </row>
     <row r="239" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -26183,7 +26183,7 @@
     </row>
     <row r="240" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -26278,7 +26278,7 @@
     </row>
     <row r="241" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B241" s="38">
         <v>63824400000</v>
@@ -26373,7 +26373,7 @@
     </row>
     <row r="242" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -26468,7 +26468,7 @@
     </row>
     <row r="243" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -26563,7 +26563,7 @@
     </row>
     <row r="244" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -26658,7 +26658,7 @@
     </row>
     <row r="245" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B245" s="38">
         <v>53116700000</v>
@@ -26753,7 +26753,7 @@
     </row>
     <row r="246" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B246" s="38">
         <v>62027300000</v>
@@ -26848,7 +26848,7 @@
     </row>
     <row r="247" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B247">
         <v>0</v>
@@ -26943,7 +26943,7 @@
     </row>
     <row r="248" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B248" s="38">
         <v>30892700000</v>
@@ -27038,7 +27038,7 @@
     </row>
     <row r="249" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B249" s="38">
         <v>31605100000</v>
@@ -27133,7 +27133,7 @@
     </row>
     <row r="250" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B250" s="38">
         <v>39774100000</v>
@@ -27228,7 +27228,7 @@
     </row>
     <row r="251" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B251" s="38">
         <v>22516500000</v>
@@ -27323,7 +27323,7 @@
     </row>
     <row r="252" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B252" s="38">
         <v>192814000000</v>
@@ -27418,7 +27418,7 @@
     </row>
     <row r="253" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B253">
         <v>0</v>
@@ -27513,7 +27513,7 @@
     </row>
     <row r="254" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B254">
         <v>0</v>
@@ -27608,7 +27608,7 @@
     </row>
     <row r="255" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B255" s="38">
         <v>1626140000000</v>
@@ -27703,7 +27703,7 @@
     </row>
     <row r="256" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B256">
         <v>0</v>
@@ -27798,7 +27798,7 @@
     </row>
     <row r="257" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B257" s="38">
         <v>0</v>
@@ -27893,7 +27893,7 @@
     </row>
     <row r="258" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B258" s="38">
         <v>0</v>
@@ -27988,7 +27988,7 @@
     </row>
     <row r="259" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B259" s="38">
         <v>0</v>
@@ -28083,7 +28083,7 @@
     </row>
     <row r="260" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B260" s="38">
         <v>0</v>
@@ -28178,7 +28178,7 @@
     </row>
     <row r="261" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B261" s="38">
         <v>0</v>
@@ -28273,7 +28273,7 @@
     </row>
     <row r="262" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B262" s="38">
         <v>0</v>
@@ -28368,7 +28368,7 @@
     </row>
     <row r="263" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B263" s="38">
         <v>0</v>
@@ -28463,7 +28463,7 @@
     </row>
     <row r="264" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B264" s="38">
         <v>0</v>
@@ -28558,7 +28558,7 @@
     </row>
     <row r="265" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B265">
         <v>0</v>
@@ -28653,7 +28653,7 @@
     </row>
     <row r="266" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B266" s="38">
         <v>0</v>
@@ -28748,7 +28748,7 @@
     </row>
     <row r="267" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B267">
         <v>0</v>
@@ -28843,7 +28843,7 @@
     </row>
     <row r="268" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B268" s="38">
         <v>0</v>
@@ -28938,7 +28938,7 @@
     </row>
     <row r="269" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B269" s="38">
         <v>0</v>
@@ -29033,7 +29033,7 @@
     </row>
     <row r="270" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B270" s="38">
         <v>0</v>
@@ -29128,7 +29128,7 @@
     </row>
     <row r="271" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B271" s="38">
         <v>0</v>
@@ -29223,7 +29223,7 @@
     </row>
     <row r="272" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B272" s="38">
         <v>0</v>
@@ -29318,7 +29318,7 @@
     </row>
     <row r="273" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B273" s="38">
         <v>0</v>
@@ -29413,7 +29413,7 @@
     </row>
     <row r="274" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B274" s="38">
         <v>0</v>
@@ -29508,7 +29508,7 @@
     </row>
     <row r="275" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B275" s="38">
         <v>0</v>
@@ -29603,7 +29603,7 @@
     </row>
     <row r="276" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B276" s="38">
         <v>0</v>
@@ -29698,7 +29698,7 @@
     </row>
     <row r="277" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B277" s="38">
         <v>0</v>
@@ -29793,7 +29793,7 @@
     </row>
     <row r="278" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B278">
         <v>0</v>
@@ -29888,7 +29888,7 @@
     </row>
     <row r="279" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B279">
         <v>0</v>
@@ -29983,7 +29983,7 @@
     </row>
     <row r="280" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B280">
         <v>0</v>
@@ -30110,7 +30110,7 @@
     </row>
     <row r="282" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B282" s="38">
         <f>SUM(B39,B64,B89,B114,B139,B164,B189,B214,B239,B264)</f>
@@ -30758,7 +30758,7 @@
   <dimension ref="A1:AE26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30769,7 +30769,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>157</v>
+        <v>448</v>
       </c>
       <c r="B1" s="1">
         <v>2021</v>
@@ -33281,7 +33281,7 @@
   <dimension ref="A1:AE26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33293,7 +33293,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>157</v>
+        <v>448</v>
       </c>
       <c r="B1" s="1">
         <v>2021</v>

</xml_diff>

<commit_message>
Remove IRA from files that had been marked as merge conflicts from develop branch
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
+++ b/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\BFoCPAbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C255099-C710-46E8-8FB3-8FE1851643E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAD32ED-9801-48CB-96E7-BFEF0B086DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2037,8 +2037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3480,8 +3480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000817FC-5CAD-42B5-92F8-1A675198574D}">
   <dimension ref="A25:H53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3563,7 +3563,7 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E35" t="s">
         <v>163</v>
@@ -3580,7 +3580,8 @@
         <v>53</v>
       </c>
       <c r="D36">
-        <v>53</v>
+        <f>19+47</f>
+        <v>66</v>
       </c>
       <c r="E36" t="s">
         <v>157</v>
@@ -3607,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3621,7 +3622,7 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3675,7 +3676,7 @@
         <v>17</v>
       </c>
       <c r="D49">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3698,7 +3699,7 @@
       </c>
       <c r="D53">
         <f>SUM(D27:D51)</f>
-        <v>194</v>
+        <v>118</v>
       </c>
       <c r="E53" t="s">
         <v>158</v>
@@ -3715,7 +3716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D869D793-4D45-441A-BEF3-5973BA28AC13}">
   <dimension ref="A1:AE300"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
@@ -31668,83 +31669,83 @@
       </c>
       <c r="L10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!L1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!L282</f>
-        <v>5.0204556960035375E-2</v>
+        <v>2.3428793248010418E-2</v>
       </c>
       <c r="M10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!M1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!M282</f>
-        <v>0.10020510951805547</v>
+        <v>4.6762384441754658E-2</v>
       </c>
       <c r="N10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!N1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!N282</f>
-        <v>0.1507214436468049</v>
+        <v>7.0336673701839242E-2</v>
       </c>
       <c r="O10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!O1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!O282</f>
-        <v>0.19945692494153741</v>
+        <v>9.3079898306049277E-2</v>
       </c>
       <c r="P10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!P1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!P282</f>
-        <v>0.24922281090780038</v>
+        <v>0.11630397842364018</v>
       </c>
       <c r="Q10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!Q1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!Q282</f>
-        <v>0.29903009479784193</v>
+        <v>0.13954737757232022</v>
       </c>
       <c r="R10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!R1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!R282</f>
-        <v>0.34856695888923633</v>
+        <v>0.16266458081497243</v>
       </c>
       <c r="S10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!S1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!S282</f>
-        <v>0.39720859939808978</v>
+        <v>0.18536401305243888</v>
       </c>
       <c r="T10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!T1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!T282</f>
-        <v>0.44540976547186162</v>
+        <v>0.20785789055353393</v>
       </c>
       <c r="U10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!U1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!U282</f>
-        <v>0.49420723985629067</v>
+        <v>0.23063004526626898</v>
       </c>
       <c r="V10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!V1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!V282</f>
-        <v>0.54117493982699039</v>
+        <v>0.25254830525258953</v>
       </c>
       <c r="W10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!W1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!W282</f>
-        <v>0.58969359265001076</v>
+        <v>0.27519034323666725</v>
       </c>
       <c r="X10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!X1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!X282</f>
-        <v>0.63835081162465501</v>
+        <v>0.29789704542483597</v>
       </c>
       <c r="Y10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!Y1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!Y282</f>
-        <v>0.68624554301044027</v>
+        <v>0.32024792007153735</v>
       </c>
       <c r="Z10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!Z1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!Z282</f>
-        <v>0.73359719115552768</v>
+        <v>0.34234535587257958</v>
       </c>
       <c r="AA10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!AA1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AA282</f>
-        <v>0.7914028342347037</v>
+        <v>0.36932132264285572</v>
       </c>
       <c r="AB10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!AB1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AB282</f>
-        <v>0.8372081665644151</v>
+        <v>0.39069714439672254</v>
       </c>
       <c r="AC10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!AC1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AC282</f>
-        <v>0.875876637615156</v>
+        <v>0.40874243088706985</v>
       </c>
       <c r="AD10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!AD1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AD282</f>
-        <v>0.9214744843594046</v>
+        <v>0.43002142603438737</v>
       </c>
       <c r="AE10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!AE1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AE282</f>
-        <v>0.97234957582328108</v>
+        <v>0.45376313538419782</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -34287,83 +34288,83 @@
       </c>
       <c r="L11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!L$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!L13</f>
-        <v>0.81198901498242848</v>
+        <v>0.85182243835893068</v>
       </c>
       <c r="M11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!M$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!M13</f>
-        <v>0.79688484453494268</v>
+        <v>0.87506977267799113</v>
       </c>
       <c r="N11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!N$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!N13</f>
-        <v>0.78432164898624812</v>
+        <v>0.89975011808234018</v>
       </c>
       <c r="O11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!O$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!O13</f>
-        <v>0.77022031086563636</v>
+        <v>0.92135788129965601</v>
       </c>
       <c r="P11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!P13</f>
-        <v>0.75748418588242916</v>
+        <v>0.94328219374038369</v>
       </c>
       <c r="Q11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Q13</f>
-        <v>0.74757043260136979</v>
+        <v>0.93093676512623413</v>
       </c>
       <c r="R11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!R13</f>
-        <v>0.73662050746216801</v>
+        <v>0.91730100929251124</v>
       </c>
       <c r="S11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!S13</f>
-        <v>0.72873104541973177</v>
+        <v>0.90747639618306242</v>
       </c>
       <c r="T11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!T13</f>
-        <v>0.71754240188738794</v>
+        <v>0.89354336838806814</v>
       </c>
       <c r="U11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!U13</f>
-        <v>0.70411100401306914</v>
+        <v>0.87681747669552024</v>
       </c>
       <c r="V11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!V13</f>
-        <v>0.69324444221904069</v>
+        <v>0.86328553181993761</v>
       </c>
       <c r="W11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!W13</f>
-        <v>0.6831113845223501</v>
+        <v>0.85066700714103993</v>
       </c>
       <c r="X11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!X13</f>
-        <v>0.67287862236327478</v>
+        <v>0.8379243221882291</v>
       </c>
       <c r="Y11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Y13</f>
-        <v>0.66494875069989612</v>
+        <v>0.8280493876640217</v>
       </c>
       <c r="Z11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Z13</f>
-        <v>0.65795128091152977</v>
+        <v>0.81933555736152774</v>
       </c>
       <c r="AA11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AA13</f>
-        <v>0.64772692249333297</v>
+        <v>0.80660333744452795</v>
       </c>
       <c r="AB11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AB13</f>
-        <v>0.63684974636887504</v>
+        <v>0.79305817472350493</v>
       </c>
       <c r="AC11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AC13</f>
-        <v>0.63085811390371926</v>
+        <v>0.78559689655934872</v>
       </c>
       <c r="AD11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AD13</f>
-        <v>0.62170295718488</v>
+        <v>0.77419613536230358</v>
       </c>
       <c r="AE11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AE13</f>
-        <v>0.60773852717324017</v>
+        <v>0.75680646780063876</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -34602,83 +34603,83 @@
       </c>
       <c r="L14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!L$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!L16</f>
-        <v>0.11700372521691103</v>
+        <v>3.5101117565073309E-2</v>
       </c>
       <c r="M14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!M$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!M16</f>
-        <v>0.23207890305552925</v>
+        <v>6.9623670916658775E-2</v>
       </c>
       <c r="N14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!N$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!N16</f>
-        <v>0.34682749060126072</v>
+        <v>0.10404824718037821</v>
       </c>
       <c r="O14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!O$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!O16</f>
-        <v>0.4593342772130351</v>
+        <v>0.13780028316391052</v>
       </c>
       <c r="P14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!P16</f>
-        <v>0.56561150307332719</v>
+        <v>0.16968345092199819</v>
       </c>
       <c r="Q14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Q16</f>
-        <v>0.55894787670852419</v>
+        <v>0.16768436301255729</v>
       </c>
       <c r="R14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!R16</f>
-        <v>0.553420054420802</v>
+        <v>0.16602601632624064</v>
       </c>
       <c r="S14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!S16</f>
-        <v>0.54758800266175711</v>
+        <v>0.16427640079852715</v>
       </c>
       <c r="T14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!T16</f>
-        <v>0.54315878163475184</v>
+        <v>0.16294763449042557</v>
       </c>
       <c r="U14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!U16</f>
-        <v>0.53734137254916481</v>
+        <v>0.16120241176474948</v>
       </c>
       <c r="V14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!V16</f>
-        <v>0.53106508933165419</v>
+        <v>0.15931952679949629</v>
       </c>
       <c r="W14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!W16</f>
-        <v>0.52619939351619838</v>
+        <v>0.15785981805485955</v>
       </c>
       <c r="X14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!X16</f>
-        <v>0.52367414147772828</v>
+        <v>0.15710224244331852</v>
       </c>
       <c r="Y14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Y16</f>
-        <v>0.5178955824889494</v>
+        <v>0.15536867474668486</v>
       </c>
       <c r="Z14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Z16</f>
-        <v>0.51128311692829631</v>
+        <v>0.15338493507848894</v>
       </c>
       <c r="AA14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AA16</f>
-        <v>0.50606654715557864</v>
+        <v>0.15181996414667362</v>
       </c>
       <c r="AB14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AB16</f>
-        <v>0.50089786197118036</v>
+        <v>0.15026935859135415</v>
       </c>
       <c r="AC14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AC16</f>
-        <v>0.49707595595226806</v>
+        <v>0.14912278678568044</v>
       </c>
       <c r="AD14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AD16</f>
-        <v>0.49364668278860729</v>
+        <v>0.14809400483658222</v>
       </c>
       <c r="AE14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AE16</f>
-        <v>0.48927518991333546</v>
+        <v>0.14678255697400067</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -34727,83 +34728,83 @@
       </c>
       <c r="L15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!L$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!L17</f>
-        <v>5.3299202415194279E-2</v>
+        <v>0</v>
       </c>
       <c r="M15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!M$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!M17</f>
-        <v>0.10553978509331634</v>
+        <v>0</v>
       </c>
       <c r="N15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!N$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!N17</f>
-        <v>0.15882400407805972</v>
+        <v>0</v>
       </c>
       <c r="O15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!O$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!O17</f>
-        <v>0.21190302754758605</v>
+        <v>0</v>
       </c>
       <c r="P15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!P17</f>
-        <v>0.26407750894138349</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Q17</f>
-        <v>0.26339454986653504</v>
+        <v>0</v>
       </c>
       <c r="R15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!R17</f>
-        <v>0.26041992571504852</v>
+        <v>0</v>
       </c>
       <c r="S15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!S17</f>
-        <v>0.25854679741500375</v>
+        <v>0</v>
       </c>
       <c r="T15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!T17</f>
-        <v>0.25805547115302419</v>
+        <v>0</v>
       </c>
       <c r="U15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!U17</f>
-        <v>0.25697029255271714</v>
+        <v>0</v>
       </c>
       <c r="V15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!V17</f>
-        <v>0.25503979786742959</v>
+        <v>0</v>
       </c>
       <c r="W15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!W17</f>
-        <v>0.25303327357778937</v>
+        <v>0</v>
       </c>
       <c r="X15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!X17</f>
-        <v>0.25230196353854722</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Y17</f>
-        <v>0.25224988882987054</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Z17</f>
-        <v>0.25282389561041013</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AA17</f>
-        <v>0.25240617748465977</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AB17</f>
-        <v>0.25126453770162882</v>
+        <v>0</v>
       </c>
       <c r="AC15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AC17</f>
-        <v>0.25110965921116141</v>
+        <v>0</v>
       </c>
       <c r="AD15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AD17</f>
-        <v>0.25074901751758777</v>
+        <v>0</v>
       </c>
       <c r="AE15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AE17</f>
-        <v>0.24825324220611877</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -35612,83 +35613,83 @@
       </c>
       <c r="L24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!L$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!L26</f>
-        <v>0.57587898701347862</v>
+        <v>0.52167861176513897</v>
       </c>
       <c r="M24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!M$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!M26</f>
-        <v>0.5749864973009432</v>
+        <v>0.46675374486781529</v>
       </c>
       <c r="N24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!N$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!N26</f>
-        <v>0.57188445068737359</v>
+        <v>0.41041119402269727</v>
       </c>
       <c r="O24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!O$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!O26</f>
-        <v>0.56363089613890405</v>
+        <v>0.35144044112190187</v>
       </c>
       <c r="P24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!P26</f>
-        <v>0.55498883677402178</v>
+        <v>0.2938176194685998</v>
       </c>
       <c r="Q24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Q26</f>
-        <v>0.54721244451833861</v>
+        <v>0.2897007059214734</v>
       </c>
       <c r="R24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!R26</f>
-        <v>0.54102812596927974</v>
+        <v>0.28642665492491282</v>
       </c>
       <c r="S24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!S26</f>
-        <v>0.53614167251941269</v>
+        <v>0.28383970898086552</v>
       </c>
       <c r="T24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!T26</f>
-        <v>0.53306039853941611</v>
+        <v>0.28220844628557323</v>
       </c>
       <c r="U24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!U26</f>
-        <v>0.5309624864163629</v>
+        <v>0.28109778692630977</v>
       </c>
       <c r="V24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!V26</f>
-        <v>0.52831617996928959</v>
+        <v>0.27969680116021212</v>
       </c>
       <c r="W24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!W26</f>
-        <v>0.5251380571598494</v>
+        <v>0.27801426555521436</v>
       </c>
       <c r="X24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!X26</f>
-        <v>0.5251380571598494</v>
+        <v>0.27801426555521436</v>
       </c>
       <c r="Y24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Y26</f>
-        <v>0.52625537217508311</v>
+        <v>0.27860578526916163</v>
       </c>
       <c r="Z24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Z26</f>
-        <v>0.52476667239523844</v>
+        <v>0.27781765009159681</v>
       </c>
       <c r="AA24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AA26</f>
-        <v>0.53058282071281171</v>
+        <v>0.28089678743619445</v>
       </c>
       <c r="AB24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AB26</f>
-        <v>0.52925825589648157</v>
+        <v>0.28019554723931378</v>
       </c>
       <c r="AC24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AC26</f>
-        <v>0.52737745185989138</v>
+        <v>0.27919982745523664</v>
       </c>
       <c r="AD24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AD26</f>
-        <v>0.52606882294708768</v>
+        <v>0.27850702391316406</v>
       </c>
       <c r="AE24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AE26</f>
-        <v>0.52236541694253236</v>
+        <v>0.27654639720487006</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Rhodium figure on BAU CCS deployment
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
+++ b/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\BFoCPAbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C255099-C710-46E8-8FB3-8FE1851643E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC28C72-98AB-48F3-BE68-E2F083CD3CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>Rhodium Group</t>
   </si>
   <si>
-    <t>The potentials below use the "Without AJP" values from Figure 3 above and are presented as MMT of capture capacity.</t>
-  </si>
-  <si>
     <t>Sources:</t>
   </si>
   <si>
@@ -1383,6 +1380,9 @@
   </si>
   <si>
     <t>Unit: Dmnl</t>
+  </si>
+  <si>
+    <t>The potentials below use the "High emissions" values from the Rhodium figure above and are presented as MMT of capture capacity.</t>
   </si>
 </sst>
 </file>
@@ -1659,50 +1659,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>227886</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>180450</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DE36599-7C54-4D1A-85C4-A8EB0343F0AE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8096250" y="171450"/>
-          <a:ext cx="5714286" cy="4200000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -1728,7 +1684,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1737,6 +1693,50 @@
         <a:xfrm>
           <a:off x="171450" y="142875"/>
           <a:ext cx="7323809" cy="4180952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>113440</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>132729</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF69BF11-C2D4-2841-45A8-4CFF0B0FA463}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8039100" y="114300"/>
+          <a:ext cx="6876190" cy="4971429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2037,7 +2037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -2051,20 +2051,20 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2074,17 +2074,17 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2092,7 +2092,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2107,27 +2107,27 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2140,18 +2140,18 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="2"/>
     </row>
@@ -2165,12 +2165,12 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2178,18 +2178,18 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2225,7 +2225,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="21"/>
@@ -2238,686 +2238,686 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="8">
         <v>0.4</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="8">
         <v>0.2</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="8">
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="8">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="8">
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="8">
         <v>0.35</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="8">
         <v>0.12</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="8">
         <v>0.7</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" s="8">
         <v>0.28999999999999998</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="8">
         <v>5</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="8">
         <v>0.1</v>
       </c>
       <c r="F13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="8">
         <v>0.3</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="8">
         <v>4.5999999999999996</v>
       </c>
       <c r="F15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" s="17">
         <v>0.9</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="8">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="8">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="8">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20" s="8">
         <v>0.8</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21" s="8">
         <v>1.2</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E22" s="8">
         <v>0.1</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E23" s="8">
         <v>0.8</v>
       </c>
       <c r="F23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="17">
         <v>1.4</v>
       </c>
       <c r="F24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="8">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" s="8">
         <v>0.6</v>
       </c>
       <c r="F26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E27" s="8">
         <v>4</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="8">
         <v>2.1</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E29" s="8">
         <v>0.3</v>
       </c>
       <c r="F29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E30" s="8">
         <v>1.4</v>
       </c>
       <c r="F30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="15"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B35" s="3">
         <f>SUM(E3:E5,E7:E9,E11:E15,E17:E20,E22:E23,E26,E29:E30)</f>
@@ -2926,7 +2926,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <f>SUM(E6,E10,E21,E25,E27:E28)</f>
@@ -2935,13 +2935,13 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" s="13"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40">
         <f>SUM(E3,E5:E6,E8,E10,E12,E15,E20,E26:E28)</f>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <f>SUM(E4,E14,E17,E29)</f>
@@ -2967,7 +2967,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42">
         <f>E7</f>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <f>SUM(E18,E21)</f>
@@ -2993,7 +2993,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44">
         <f>E30</f>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B45">
         <f>E23</f>
@@ -3019,7 +3019,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B46">
         <f>SUM(E11,E13,E25)</f>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47">
         <f>SUM(E9,E22)</f>
@@ -3045,7 +3045,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B48">
         <f>E19</f>
@@ -3091,14 +3091,14 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3125,7 +3125,7 @@
         <v>250</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3136,30 +3136,30 @@
         <v>272</v>
       </c>
       <c r="C6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -3171,7 +3171,7 @@
         <v>0.55339805825242716</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -3183,7 +3183,7 @@
         <v>0.3300970873786408</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -3195,7 +3195,7 @@
         <v>2.9126213592233007E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -3207,7 +3207,7 @@
         <v>2.9126213592233007E-2</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3219,7 +3219,7 @@
         <v>1.9417475728155338E-2</v>
       </c>
       <c r="C15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3231,23 +3231,23 @@
         <v>3.8834951456310676E-2</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3257,23 +3257,23 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3281,12 +3281,12 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -3294,12 +3294,12 @@
         <v>80</v>
       </c>
       <c r="B29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -3308,13 +3308,13 @@
         <v>82.524271844660205</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B33" s="32"/>
       <c r="C33" s="32"/>
@@ -3326,30 +3326,30 @@
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="28"/>
       <c r="B34" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F34" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B35" s="2">
         <f>B5*B11</f>
@@ -3380,7 +3380,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B37" s="25">
         <v>0</v>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -3451,7 +3451,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -3462,7 +3462,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3480,8 +3480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000817FC-5CAD-42B5-92F8-1A675198574D}">
   <dimension ref="A25:H53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3491,7 +3491,7 @@
   <sheetData>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>27</v>
+        <v>448</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -3566,7 +3566,7 @@
         <v>60</v>
       </c>
       <c r="E35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3583,7 +3583,7 @@
         <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3672,10 +3672,10 @@
         <v>14</v>
       </c>
       <c r="C49">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D49">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3690,18 +3690,18 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C53">
         <f>SUM(C27:C51)</f>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D53">
         <f>SUM(D27:D51)</f>
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E53" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -3726,12 +3726,12 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3">
         <v>2021</v>
@@ -3826,7 +3826,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" s="38">
         <v>8000000000000</v>
@@ -3921,7 +3921,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" s="38">
         <v>2200000000000</v>
@@ -4016,7 +4016,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" s="38">
         <v>33800000000000</v>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B7" s="38">
         <v>0</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8" s="38">
         <v>0</v>
@@ -4301,7 +4301,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B9" s="38">
         <v>0</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" s="38">
         <v>0</v>
@@ -4491,7 +4491,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" s="38">
         <v>0</v>
@@ -4586,7 +4586,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" s="38">
         <v>2300000000000</v>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13" s="38">
         <v>49700000000000</v>
@@ -4776,7 +4776,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14" s="38">
         <v>0</v>
@@ -4871,7 +4871,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4966,7 +4966,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B16" s="38">
         <v>63800000000000</v>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B17" s="38">
         <v>36800000000000</v>
@@ -5156,7 +5156,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B18" s="38">
         <v>4400000000000</v>
@@ -5251,7 +5251,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B19" s="38">
         <v>0</v>
@@ -5346,7 +5346,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B20" s="38">
         <v>1007000000</v>
@@ -5441,7 +5441,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B21" s="38">
         <v>0</v>
@@ -5536,7 +5536,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B22" s="38">
         <v>0</v>
@@ -5631,7 +5631,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B23" s="38">
         <v>0</v>
@@ -5726,7 +5726,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B24" s="38">
         <v>0</v>
@@ -5821,7 +5821,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B25" s="38">
         <v>0</v>
@@ -5916,7 +5916,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B26" s="38">
         <v>27500000000000</v>
@@ -6011,7 +6011,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -6106,7 +6106,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B28" s="38">
         <v>0</v>
@@ -6233,7 +6233,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30">
         <v>2021</v>
@@ -6328,7 +6328,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B31" s="38">
         <v>0</v>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B32" s="38">
         <v>0</v>
@@ -6518,7 +6518,7 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B33" s="38">
         <v>0</v>
@@ -6613,7 +6613,7 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B34" s="38">
         <v>0</v>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B35" s="38">
         <v>0</v>
@@ -6803,7 +6803,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B36" s="38">
         <v>0</v>
@@ -6898,7 +6898,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B37" s="38">
         <v>0</v>
@@ -6993,7 +6993,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B38" s="38">
         <v>0</v>
@@ -7088,7 +7088,7 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -7183,7 +7183,7 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -7278,7 +7278,7 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -7373,7 +7373,7 @@
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -7468,7 +7468,7 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -7563,7 +7563,7 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -7658,7 +7658,7 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -7753,7 +7753,7 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -7848,7 +7848,7 @@
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -7943,7 +7943,7 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -8038,7 +8038,7 @@
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -8133,7 +8133,7 @@
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -8228,7 +8228,7 @@
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -8323,7 +8323,7 @@
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -8418,7 +8418,7 @@
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -8513,7 +8513,7 @@
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -8608,7 +8608,7 @@
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -8703,7 +8703,7 @@
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -8798,7 +8798,7 @@
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -8893,7 +8893,7 @@
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B58" s="38">
         <v>19502000000</v>
@@ -8988,7 +8988,7 @@
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B59" s="38">
         <v>2092490000000</v>
@@ -9083,7 +9083,7 @@
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B60" s="38">
         <v>11632100000000</v>
@@ -9178,7 +9178,7 @@
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B61" s="38">
         <v>106076000000</v>
@@ -9273,7 +9273,7 @@
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -9368,7 +9368,7 @@
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B63" s="38">
         <v>5190830000000</v>
@@ -9463,7 +9463,7 @@
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B64" s="38">
         <v>2272080000000</v>
@@ -9558,7 +9558,7 @@
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B65" s="38">
         <v>9334890000000</v>
@@ -9653,7 +9653,7 @@
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -9748,7 +9748,7 @@
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -9843,7 +9843,7 @@
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B68" s="38">
         <v>16366600000000</v>
@@ -9938,7 +9938,7 @@
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B69" s="38">
         <v>3431200000000</v>
@@ -10033,7 +10033,7 @@
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B70" s="38">
         <v>91263500000</v>
@@ -10128,7 +10128,7 @@
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -10223,7 +10223,7 @@
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -10318,7 +10318,7 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -10413,7 +10413,7 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -10508,7 +10508,7 @@
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -10603,7 +10603,7 @@
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -10698,7 +10698,7 @@
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B77" s="38">
         <v>331286000000</v>
@@ -10793,7 +10793,7 @@
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -10888,7 +10888,7 @@
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -10983,7 +10983,7 @@
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -11078,7 +11078,7 @@
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B81" s="38">
         <v>4960930000000</v>
@@ -11173,7 +11173,7 @@
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B82" s="38">
         <v>7932630000000</v>
@@ -11268,7 +11268,7 @@
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B83" s="38">
         <v>108060000000000</v>
@@ -11363,7 +11363,7 @@
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B84" s="38">
         <v>11110900000000</v>
@@ -11458,7 +11458,7 @@
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B85" s="38">
         <v>48585900000000</v>
@@ -11553,7 +11553,7 @@
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B86" s="38">
         <v>5537710000000</v>
@@ -11648,7 +11648,7 @@
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B87" s="38">
         <v>3097290000000</v>
@@ -11743,7 +11743,7 @@
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B88" s="38">
         <v>29767700000000</v>
@@ -11838,7 +11838,7 @@
     </row>
     <row r="89" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B89" s="38">
         <v>43963500000000</v>
@@ -11933,7 +11933,7 @@
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B90" s="38">
         <v>108608000000000</v>
@@ -12028,7 +12028,7 @@
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B91" s="38">
         <v>4303610000000</v>
@@ -12123,7 +12123,7 @@
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B92" s="38">
         <v>5723100000000</v>
@@ -12218,7 +12218,7 @@
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B93" s="38">
         <v>4350300000000</v>
@@ -12313,7 +12313,7 @@
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B94" s="38">
         <v>0</v>
@@ -12408,7 +12408,7 @@
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B95" s="38">
         <v>10152700000000</v>
@@ -12503,7 +12503,7 @@
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B96" s="38">
         <v>5876500000000</v>
@@ -12598,7 +12598,7 @@
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B97" s="38">
         <v>1637870000000</v>
@@ -12693,7 +12693,7 @@
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B98" s="38">
         <v>1650940000000</v>
@@ -12788,7 +12788,7 @@
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B99" s="38">
         <v>2892370000000</v>
@@ -12883,7 +12883,7 @@
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B100" s="38">
         <v>5139370000000</v>
@@ -12978,7 +12978,7 @@
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B101" s="38">
         <v>2909440000000</v>
@@ -13073,7 +13073,7 @@
     </row>
     <row r="102" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B102" s="38">
         <v>17295000000000</v>
@@ -13168,7 +13168,7 @@
     </row>
     <row r="103" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B103" s="38">
         <v>55637100000000</v>
@@ -13263,7 +13263,7 @@
     </row>
     <row r="104" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B104" s="38">
         <v>0</v>
@@ -13358,7 +13358,7 @@
     </row>
     <row r="105" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B105" s="38">
         <v>11695200000000</v>
@@ -13453,7 +13453,7 @@
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B106" s="38">
         <v>0</v>
@@ -13548,7 +13548,7 @@
     </row>
     <row r="107" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B107" s="38">
         <v>0</v>
@@ -13643,7 +13643,7 @@
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B108" s="38">
         <v>0</v>
@@ -13738,7 +13738,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -13833,7 +13833,7 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B110" s="38">
         <v>0</v>
@@ -13928,7 +13928,7 @@
     </row>
     <row r="111" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -14023,7 +14023,7 @@
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B112" s="38">
         <v>0</v>
@@ -14118,7 +14118,7 @@
     </row>
     <row r="113" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B113" s="38">
         <v>0</v>
@@ -14213,7 +14213,7 @@
     </row>
     <row r="114" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B114" s="38">
         <v>0</v>
@@ -14308,7 +14308,7 @@
     </row>
     <row r="115" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B115" s="38">
         <v>0</v>
@@ -14403,7 +14403,7 @@
     </row>
     <row r="116" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B116" s="38">
         <v>0</v>
@@ -14498,7 +14498,7 @@
     </row>
     <row r="117" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B117" s="38">
         <v>0</v>
@@ -14593,7 +14593,7 @@
     </row>
     <row r="118" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B118" s="38">
         <v>0</v>
@@ -14688,7 +14688,7 @@
     </row>
     <row r="119" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B119" s="38">
         <v>0</v>
@@ -14783,7 +14783,7 @@
     </row>
     <row r="120" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B120" s="38">
         <v>0</v>
@@ -14878,7 +14878,7 @@
     </row>
     <row r="121" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B121" s="38">
         <v>0</v>
@@ -14973,7 +14973,7 @@
     </row>
     <row r="122" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B122" s="38">
         <v>0</v>
@@ -15068,7 +15068,7 @@
     </row>
     <row r="123" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B123" s="38">
         <v>0</v>
@@ -15163,7 +15163,7 @@
     </row>
     <row r="124" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -15258,7 +15258,7 @@
     </row>
     <row r="125" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -15353,7 +15353,7 @@
     </row>
     <row r="126" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -15448,7 +15448,7 @@
     </row>
     <row r="127" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -15543,7 +15543,7 @@
     </row>
     <row r="128" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -15638,7 +15638,7 @@
     </row>
     <row r="129" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -15733,7 +15733,7 @@
     </row>
     <row r="130" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -15828,7 +15828,7 @@
     </row>
     <row r="131" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B131" s="38">
         <v>35940700000000</v>
@@ -15923,7 +15923,7 @@
     </row>
     <row r="132" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B132" s="38">
         <v>2761920000000</v>
@@ -16018,7 +16018,7 @@
     </row>
     <row r="133" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B133" s="38">
         <v>8379870000000</v>
@@ -16113,7 +16113,7 @@
     </row>
     <row r="134" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B134" s="38">
         <v>8506080000000</v>
@@ -16208,7 +16208,7 @@
     </row>
     <row r="135" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B135" s="38">
         <v>2368720000000</v>
@@ -16303,7 +16303,7 @@
     </row>
     <row r="136" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B136" s="38">
         <v>982499000000</v>
@@ -16398,7 +16398,7 @@
     </row>
     <row r="137" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B137" s="38">
         <v>612997000000</v>
@@ -16493,7 +16493,7 @@
     </row>
     <row r="138" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B138" s="38">
         <v>344397000000</v>
@@ -16588,7 +16588,7 @@
     </row>
     <row r="139" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -16683,7 +16683,7 @@
     </row>
     <row r="140" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B140" s="38">
         <v>85828500000</v>
@@ -16778,7 +16778,7 @@
     </row>
     <row r="141" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -16873,7 +16873,7 @@
     </row>
     <row r="142" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -16968,7 +16968,7 @@
     </row>
     <row r="143" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B143" s="38">
         <v>1625460000000</v>
@@ -17063,7 +17063,7 @@
     </row>
     <row r="144" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B144" s="38">
         <v>309260000000</v>
@@ -17158,7 +17158,7 @@
     </row>
     <row r="145" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B145" s="38">
         <v>922309000000</v>
@@ -17253,7 +17253,7 @@
     </row>
     <row r="146" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -17348,7 +17348,7 @@
     </row>
     <row r="147" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -17443,7 +17443,7 @@
     </row>
     <row r="148" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B148" s="38">
         <v>0</v>
@@ -17538,7 +17538,7 @@
     </row>
     <row r="149" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B149" s="38">
         <v>86011600000</v>
@@ -17633,7 +17633,7 @@
     </row>
     <row r="150" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B150" s="38">
         <v>163681000000</v>
@@ -17728,7 +17728,7 @@
     </row>
     <row r="151" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B151" s="38">
         <v>92660900000</v>
@@ -17823,7 +17823,7 @@
     </row>
     <row r="152" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B152" s="38">
         <v>3068450000000</v>
@@ -17918,7 +17918,7 @@
     </row>
     <row r="153" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B153" s="38">
         <v>0</v>
@@ -18013,7 +18013,7 @@
     </row>
     <row r="154" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B154" s="38">
         <v>0</v>
@@ -18108,7 +18108,7 @@
     </row>
     <row r="155" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B155" s="38">
         <v>44833300000000</v>
@@ -18203,7 +18203,7 @@
     </row>
     <row r="156" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B156" s="38">
         <v>0</v>
@@ -18298,7 +18298,7 @@
     </row>
     <row r="157" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -18393,7 +18393,7 @@
     </row>
     <row r="158" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -18488,7 +18488,7 @@
     </row>
     <row r="159" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -18583,7 +18583,7 @@
     </row>
     <row r="160" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B160" s="38">
         <v>0</v>
@@ -18678,7 +18678,7 @@
     </row>
     <row r="161" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B161" s="38">
         <v>0</v>
@@ -18773,7 +18773,7 @@
     </row>
     <row r="162" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B162" s="38">
         <v>0</v>
@@ -18868,7 +18868,7 @@
     </row>
     <row r="163" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B163" s="38">
         <v>0</v>
@@ -18963,7 +18963,7 @@
     </row>
     <row r="164" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B164" s="38">
         <v>0</v>
@@ -19058,7 +19058,7 @@
     </row>
     <row r="165" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B165" s="38">
         <v>0</v>
@@ -19153,7 +19153,7 @@
     </row>
     <row r="166" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B166" s="38">
         <v>0</v>
@@ -19248,7 +19248,7 @@
     </row>
     <row r="167" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B167" s="38">
         <v>0</v>
@@ -19343,7 +19343,7 @@
     </row>
     <row r="168" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B168" s="38">
         <v>0</v>
@@ -19438,7 +19438,7 @@
     </row>
     <row r="169" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -19533,7 +19533,7 @@
     </row>
     <row r="170" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -19628,7 +19628,7 @@
     </row>
     <row r="171" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -19723,7 +19723,7 @@
     </row>
     <row r="172" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B172" s="38">
         <v>0</v>
@@ -19818,7 +19818,7 @@
     </row>
     <row r="173" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B173" s="38">
         <v>0</v>
@@ -19913,7 +19913,7 @@
     </row>
     <row r="174" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B174" s="38">
         <v>0</v>
@@ -20008,7 +20008,7 @@
     </row>
     <row r="175" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B175" s="38">
         <v>0</v>
@@ -20103,7 +20103,7 @@
     </row>
     <row r="176" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B176" s="38">
         <v>0</v>
@@ -20198,7 +20198,7 @@
     </row>
     <row r="177" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B177" s="38">
         <v>0</v>
@@ -20293,7 +20293,7 @@
     </row>
     <row r="178" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B178" s="38">
         <v>0</v>
@@ -20388,7 +20388,7 @@
     </row>
     <row r="179" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B179" s="38">
         <v>0</v>
@@ -20483,7 +20483,7 @@
     </row>
     <row r="180" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B180" s="38">
         <v>0</v>
@@ -20578,7 +20578,7 @@
     </row>
     <row r="181" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -20673,7 +20673,7 @@
     </row>
     <row r="182" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -20768,7 +20768,7 @@
     </row>
     <row r="183" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B183" s="38">
         <v>0</v>
@@ -20863,7 +20863,7 @@
     </row>
     <row r="184" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -20958,7 +20958,7 @@
     </row>
     <row r="185" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B185">
         <v>0</v>
@@ -21053,7 +21053,7 @@
     </row>
     <row r="186" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -21148,7 +21148,7 @@
     </row>
     <row r="187" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -21243,7 +21243,7 @@
     </row>
     <row r="188" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -21338,7 +21338,7 @@
     </row>
     <row r="189" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B189" s="38">
         <v>132433000000000</v>
@@ -21433,7 +21433,7 @@
     </row>
     <row r="190" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -21528,7 +21528,7 @@
     </row>
     <row r="191" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -21623,7 +21623,7 @@
     </row>
     <row r="192" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -21718,7 +21718,7 @@
     </row>
     <row r="193" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B193">
         <v>0</v>
@@ -21813,7 +21813,7 @@
     </row>
     <row r="194" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -21908,7 +21908,7 @@
     </row>
     <row r="195" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B195">
         <v>0</v>
@@ -22003,7 +22003,7 @@
     </row>
     <row r="196" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B196" s="38">
         <v>0</v>
@@ -22098,7 +22098,7 @@
     </row>
     <row r="197" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -22193,7 +22193,7 @@
     </row>
     <row r="198" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -22288,7 +22288,7 @@
     </row>
     <row r="199" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -22383,7 +22383,7 @@
     </row>
     <row r="200" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -22478,7 +22478,7 @@
     </row>
     <row r="201" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B201">
         <v>0</v>
@@ -22573,7 +22573,7 @@
     </row>
     <row r="202" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -22668,7 +22668,7 @@
     </row>
     <row r="203" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -22763,7 +22763,7 @@
     </row>
     <row r="204" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -22858,7 +22858,7 @@
     </row>
     <row r="205" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -22953,7 +22953,7 @@
     </row>
     <row r="206" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B206" s="38">
         <v>16453000000</v>
@@ -23048,7 +23048,7 @@
     </row>
     <row r="207" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B207" s="38">
         <v>59246200000</v>
@@ -23143,7 +23143,7 @@
     </row>
     <row r="208" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B208" s="38">
         <v>322572000000</v>
@@ -23238,7 +23238,7 @@
     </row>
     <row r="209" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B209">
         <v>0</v>
@@ -23333,7 +23333,7 @@
     </row>
     <row r="210" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B210" s="38">
         <v>28550500000</v>
@@ -23428,7 +23428,7 @@
     </row>
     <row r="211" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B211" s="38">
         <v>14411100000</v>
@@ -23523,7 +23523,7 @@
     </row>
     <row r="212" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -23618,7 +23618,7 @@
     </row>
     <row r="213" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B213" s="38">
         <v>2067700000000</v>
@@ -23713,7 +23713,7 @@
     </row>
     <row r="214" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -23808,7 +23808,7 @@
     </row>
     <row r="215" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B215" s="38">
         <v>263361000000</v>
@@ -23903,7 +23903,7 @@
     </row>
     <row r="216" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B216" s="38">
         <v>8486300</v>
@@ -23998,7 +23998,7 @@
     </row>
     <row r="217" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B217">
         <v>0</v>
@@ -24093,7 +24093,7 @@
     </row>
     <row r="218" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -24188,7 +24188,7 @@
     </row>
     <row r="219" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -24283,7 +24283,7 @@
     </row>
     <row r="220" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B220" s="38">
         <v>12398800000</v>
@@ -24378,7 +24378,7 @@
     </row>
     <row r="221" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B221" s="38">
         <v>393749000</v>
@@ -24473,7 +24473,7 @@
     </row>
     <row r="222" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B222" s="38">
         <v>3679900</v>
@@ -24568,7 +24568,7 @@
     </row>
     <row r="223" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -24663,7 +24663,7 @@
     </row>
     <row r="224" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B224" s="38">
         <v>21628800</v>
@@ -24758,7 +24758,7 @@
     </row>
     <row r="225" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B225" s="38">
         <v>178015000000</v>
@@ -24853,7 +24853,7 @@
     </row>
     <row r="226" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B226" s="38">
         <v>100776000000</v>
@@ -24948,7 +24948,7 @@
     </row>
     <row r="227" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B227" s="38">
         <v>45007600000</v>
@@ -25043,7 +25043,7 @@
     </row>
     <row r="228" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -25138,7 +25138,7 @@
     </row>
     <row r="229" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -25233,7 +25233,7 @@
     </row>
     <row r="230" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -25328,7 +25328,7 @@
     </row>
     <row r="231" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B231" s="38">
         <v>5608430000000</v>
@@ -25423,7 +25423,7 @@
     </row>
     <row r="232" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -25518,7 +25518,7 @@
     </row>
     <row r="233" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -25613,7 +25613,7 @@
     </row>
     <row r="234" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -25708,7 +25708,7 @@
     </row>
     <row r="235" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B235" s="38">
         <v>257088000000</v>
@@ -25803,7 +25803,7 @@
     </row>
     <row r="236" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B236" s="38">
         <v>61737800000</v>
@@ -25898,7 +25898,7 @@
     </row>
     <row r="237" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B237" s="38">
         <v>96430100000</v>
@@ -25993,7 +25993,7 @@
     </row>
     <row r="238" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B238" s="38">
         <v>35762800000</v>
@@ -26088,7 +26088,7 @@
     </row>
     <row r="239" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -26183,7 +26183,7 @@
     </row>
     <row r="240" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -26278,7 +26278,7 @@
     </row>
     <row r="241" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B241" s="38">
         <v>63824400000</v>
@@ -26373,7 +26373,7 @@
     </row>
     <row r="242" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -26468,7 +26468,7 @@
     </row>
     <row r="243" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -26563,7 +26563,7 @@
     </row>
     <row r="244" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -26658,7 +26658,7 @@
     </row>
     <row r="245" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B245" s="38">
         <v>53116700000</v>
@@ -26753,7 +26753,7 @@
     </row>
     <row r="246" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B246" s="38">
         <v>62027300000</v>
@@ -26848,7 +26848,7 @@
     </row>
     <row r="247" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B247">
         <v>0</v>
@@ -26943,7 +26943,7 @@
     </row>
     <row r="248" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B248" s="38">
         <v>30892700000</v>
@@ -27038,7 +27038,7 @@
     </row>
     <row r="249" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B249" s="38">
         <v>31605100000</v>
@@ -27133,7 +27133,7 @@
     </row>
     <row r="250" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B250" s="38">
         <v>39774100000</v>
@@ -27228,7 +27228,7 @@
     </row>
     <row r="251" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B251" s="38">
         <v>22516500000</v>
@@ -27323,7 +27323,7 @@
     </row>
     <row r="252" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B252" s="38">
         <v>192814000000</v>
@@ -27418,7 +27418,7 @@
     </row>
     <row r="253" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B253">
         <v>0</v>
@@ -27513,7 +27513,7 @@
     </row>
     <row r="254" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B254">
         <v>0</v>
@@ -27608,7 +27608,7 @@
     </row>
     <row r="255" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B255" s="38">
         <v>1626140000000</v>
@@ -27703,7 +27703,7 @@
     </row>
     <row r="256" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B256">
         <v>0</v>
@@ -27798,7 +27798,7 @@
     </row>
     <row r="257" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B257" s="38">
         <v>0</v>
@@ -27893,7 +27893,7 @@
     </row>
     <row r="258" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B258" s="38">
         <v>0</v>
@@ -27988,7 +27988,7 @@
     </row>
     <row r="259" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B259" s="38">
         <v>0</v>
@@ -28083,7 +28083,7 @@
     </row>
     <row r="260" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B260" s="38">
         <v>0</v>
@@ -28178,7 +28178,7 @@
     </row>
     <row r="261" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B261" s="38">
         <v>0</v>
@@ -28273,7 +28273,7 @@
     </row>
     <row r="262" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B262" s="38">
         <v>0</v>
@@ -28368,7 +28368,7 @@
     </row>
     <row r="263" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B263" s="38">
         <v>0</v>
@@ -28463,7 +28463,7 @@
     </row>
     <row r="264" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B264" s="38">
         <v>0</v>
@@ -28558,7 +28558,7 @@
     </row>
     <row r="265" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B265">
         <v>0</v>
@@ -28653,7 +28653,7 @@
     </row>
     <row r="266" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B266" s="38">
         <v>0</v>
@@ -28748,7 +28748,7 @@
     </row>
     <row r="267" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B267">
         <v>0</v>
@@ -28843,7 +28843,7 @@
     </row>
     <row r="268" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B268" s="38">
         <v>0</v>
@@ -28938,7 +28938,7 @@
     </row>
     <row r="269" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B269" s="38">
         <v>0</v>
@@ -29033,7 +29033,7 @@
     </row>
     <row r="270" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B270" s="38">
         <v>0</v>
@@ -29128,7 +29128,7 @@
     </row>
     <row r="271" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B271" s="38">
         <v>0</v>
@@ -29223,7 +29223,7 @@
     </row>
     <row r="272" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B272" s="38">
         <v>0</v>
@@ -29318,7 +29318,7 @@
     </row>
     <row r="273" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B273" s="38">
         <v>0</v>
@@ -29413,7 +29413,7 @@
     </row>
     <row r="274" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B274" s="38">
         <v>0</v>
@@ -29508,7 +29508,7 @@
     </row>
     <row r="275" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B275" s="38">
         <v>0</v>
@@ -29603,7 +29603,7 @@
     </row>
     <row r="276" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B276" s="38">
         <v>0</v>
@@ -29698,7 +29698,7 @@
     </row>
     <row r="277" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B277" s="38">
         <v>0</v>
@@ -29793,7 +29793,7 @@
     </row>
     <row r="278" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B278">
         <v>0</v>
@@ -29888,7 +29888,7 @@
     </row>
     <row r="279" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B279">
         <v>0</v>
@@ -29983,7 +29983,7 @@
     </row>
     <row r="280" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B280">
         <v>0</v>
@@ -30110,7 +30110,7 @@
     </row>
     <row r="282" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B282" s="38">
         <f>SUM(B39,B64,B89,B114,B139,B164,B189,B214,B239,B264)</f>
@@ -30769,7 +30769,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B1" s="1">
         <v>2021</v>
@@ -33293,7 +33293,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B1" s="1">
         <v>2021</v>
@@ -35572,7 +35572,7 @@
       </c>
       <c r="B24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!B$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!B26</f>
-        <v>0.43251437513148949</v>
+        <v>0.43648239692168667</v>
       </c>
       <c r="C24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!C$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!C26</f>
@@ -35580,115 +35580,115 @@
       </c>
       <c r="D24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!D$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!D26</f>
-        <v>0.43663426971115138</v>
+        <v>0.43283744997453266</v>
       </c>
       <c r="E24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!E$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!E26</f>
-        <v>0.48081518704965481</v>
+        <v>0.47266577709966062</v>
       </c>
       <c r="F24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!F$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!F26</f>
-        <v>0.49693611241554458</v>
+        <v>0.4846153823556551</v>
       </c>
       <c r="G24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!G$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!G26</f>
-        <v>0.50413391596767088</v>
+        <v>0.487871531581617</v>
       </c>
       <c r="H24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!H$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!H26</f>
-        <v>0.5245388380871896</v>
+        <v>0.50388770272942629</v>
       </c>
       <c r="I24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!I$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!I26</f>
-        <v>0.54434681120317785</v>
+        <v>0.51922311222456963</v>
       </c>
       <c r="J24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!J$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!J26</f>
-        <v>0.56013275560193287</v>
+        <v>0.53065208425446275</v>
       </c>
       <c r="K24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!K$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!K26</f>
-        <v>0.5732097912451658</v>
+        <v>0.53949156823074429</v>
       </c>
       <c r="L24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!L$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!L26</f>
-        <v>0.57587898701347862</v>
+        <v>0.54200375248327404</v>
       </c>
       <c r="M24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!M$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!M26</f>
-        <v>0.5749864973009432</v>
+        <v>0.54116376216559359</v>
       </c>
       <c r="N24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!N$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!N26</f>
-        <v>0.57188445068737359</v>
+        <v>0.53824418888223391</v>
       </c>
       <c r="O24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!O$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!O26</f>
-        <v>0.56363089613890405</v>
+        <v>0.53047613754249789</v>
       </c>
       <c r="P24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!P26</f>
-        <v>0.55498883677402178</v>
+        <v>0.52234243461084406</v>
       </c>
       <c r="Q24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Q26</f>
-        <v>0.54721244451833861</v>
+        <v>0.51502347719373043</v>
       </c>
       <c r="R24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!R26</f>
-        <v>0.54102812596927974</v>
+        <v>0.50920294208873385</v>
       </c>
       <c r="S24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!S26</f>
-        <v>0.53614167251941269</v>
+        <v>0.50460392707709434</v>
       </c>
       <c r="T24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!T26</f>
-        <v>0.53306039853941611</v>
+        <v>0.50170390450768576</v>
       </c>
       <c r="U24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!U26</f>
-        <v>0.5309624864163629</v>
+        <v>0.49972939898010627</v>
       </c>
       <c r="V24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!V26</f>
-        <v>0.52831617996928959</v>
+        <v>0.49723875761815489</v>
       </c>
       <c r="W24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!W26</f>
-        <v>0.5251380571598494</v>
+        <v>0.49424758320927004</v>
       </c>
       <c r="X24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!X26</f>
-        <v>0.5251380571598494</v>
+        <v>0.49424758320927004</v>
       </c>
       <c r="Y24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Y26</f>
-        <v>0.52625537217508311</v>
+        <v>0.49529917381184291</v>
       </c>
       <c r="Z24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Z26</f>
-        <v>0.52476667239523844</v>
+        <v>0.49389804460728326</v>
       </c>
       <c r="AA24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AA26</f>
-        <v>0.53058282071281171</v>
+        <v>0.49937206655323457</v>
       </c>
       <c r="AB24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AB26</f>
-        <v>0.52925825589648157</v>
+        <v>0.49812541731433563</v>
       </c>
       <c r="AC24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AC26</f>
-        <v>0.52737745185989138</v>
+        <v>0.49635524880930953</v>
       </c>
       <c r="AD24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AD26</f>
-        <v>0.52606882294708768</v>
+        <v>0.49512359806784723</v>
       </c>
       <c r="AE24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$49:$D$49,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AE26</f>
-        <v>0.52236541694253236</v>
+        <v>0.49163803947532458</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Unpushed change to BFoCPAbI file
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
+++ b/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BFoCPAbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DAC2E32-3987-4484-9D1D-AD71DDAD2B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949B2F3E-2E0D-4E7D-88A1-5C6936F29631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1571,7 +1571,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1631,7 +1631,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3075,8 +3074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED05A5AB-C865-4DF5-BD35-041C1CC241DD}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3481,8 +3480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000817FC-5CAD-42B5-92F8-1A675198574D}">
   <dimension ref="A25:H53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30756,7 +30755,7 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AE29"/>
+  <dimension ref="A1:AE26"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P10" sqref="P10"/>
@@ -31628,59 +31627,59 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!B1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!B282</f>
         <v>0</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!C1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!C282</f>
         <v>0</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!D1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!D282</f>
         <v>0</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!E1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!E282</f>
         <v>0</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!F1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!F282</f>
         <v>0</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!G1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!G282</f>
         <v>0</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!H1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!H282</f>
         <v>0</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!I1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!I282</f>
         <v>0</v>
       </c>
-      <c r="J10" s="39">
+      <c r="J10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!J1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!J282</f>
         <v>0</v>
       </c>
-      <c r="K10" s="39">
+      <c r="K10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!K1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!K282</f>
         <v>0</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!L1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!L282</f>
         <v>5.9003997687245381E-2</v>
       </c>
-      <c r="M10" s="39">
+      <c r="M10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!M1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!M282</f>
         <v>0.11802503260835458</v>
       </c>
-      <c r="N10" s="39">
+      <c r="N10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!N1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!N282</f>
         <v>0.1776797461581178</v>
       </c>
-      <c r="O10" s="39">
+      <c r="O10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!O1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!O282</f>
         <v>0.23449511394460765</v>
       </c>
@@ -33268,24 +33267,6 @@
       <c r="AE26">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="39"/>
-      <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
-      <c r="X29" s="39"/>
-      <c r="Y29" s="39"/>
-      <c r="Z29" s="39"/>
-      <c r="AA29" s="39"/>
-      <c r="AB29" s="39"/>
-      <c r="AC29" s="39"/>
-      <c r="AD29" s="39"/>
-      <c r="AE29" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33300,7 +33281,7 @@
   </sheetPr>
   <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrections to no IRA trajectory to align 2021 and 2022 values
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
+++ b/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\ccs\BFoCPAbI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BFoCPAbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EDB600F-0904-4D0E-9995-6ACA46BB5C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3720AF4C-A72F-4D04-A4EA-C78BF937958D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7875" yWindow="4455" windowWidth="37485" windowHeight="17055" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2037,7 +2037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -3480,7 +3480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000817FC-5CAD-42B5-92F8-1A675198574D}">
   <dimension ref="A25:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -33282,7 +33282,7 @@
   <dimension ref="A1:AE26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34251,8 +34251,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="38">
-        <f>MAX(TREND('Current and Planned Capacity'!$B$36:$C$36,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!C$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!C13</f>
-        <v>3.1900778141544787E-2</v>
+        <v>9.1697982546572812E-3</v>
       </c>
       <c r="D11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$36:$C$36,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!D$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!D13</f>
@@ -35572,12 +35571,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="38">
-        <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!B$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!B26</f>
-        <v>0.43251437513148949</v>
+        <v>0.44456540427208824</v>
       </c>
       <c r="C24" s="38">
-        <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!C$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!C26</f>
-        <v>0.40684111563938835</v>
+        <v>0.45264841162248987</v>
       </c>
       <c r="D24" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$49:$C$49,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!D$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!D26</f>

</xml_diff>

<commit_message>
Update BAU CCS amounts for latest BAU trajectory
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
+++ b/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BFoCPAbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949B2F3E-2E0D-4E7D-88A1-5C6936F29631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC5CB6F-314F-43D3-8989-23618BD71A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -560,829 +560,829 @@
     <t>Time (Year)</t>
   </si>
   <si>
-    <t>Process Emissions before CCS[agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Process Emissions before CCS[construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heat if,construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,construction 41T43,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,agriculture and forestry 01T03,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,coal mining 05,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,oil and gas extraction 06,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,other mining and quarrying 07T08,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,food beverage and tobacco 10T12,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,textiles apparel and leather 13T15,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,wood products 16,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,pulp paper and printing 17T18,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,refined petroleum and coke 19,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,chemicals 20,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,rubber and plastic products 22,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,glass and glass products 231,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,cement and other nonmetallic minerals 239,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,iron and steel 241,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,other metals 242,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,metal products except machinery and vehicles 25,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,computers and electronics 26,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,appliances and electrical equipment 27,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,other machinery 28,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,road vehicles 29,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,nonroad vehicles 30,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,other manufacturing 31T33,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,energy pipelines and gas processing 352T353,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,water and waste 36T39,CO2] : NoSettings</t>
-  </si>
-  <si>
-    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,construction 41T43,CO2] : NoSettings</t>
+    <t>Process Emissions before CCS[agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Process Emissions before CCS[construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[electricity if,construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hard coal if,construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[natural gas if,construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[biomass if,construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[petroleum diesel if,construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heat if,construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[crude oil if,construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[heavy or residual fuel oil if,construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[LPG propane or butane if,construction 41T43,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,agriculture and forestry 01T03,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,coal mining 05,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,oil and gas extraction 06,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,other mining and quarrying 07T08,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,food beverage and tobacco 10T12,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,textiles apparel and leather 13T15,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,wood products 16,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,pulp paper and printing 17T18,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,refined petroleum and coke 19,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,chemicals 20,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,rubber and plastic products 22,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,glass and glass products 231,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,cement and other nonmetallic minerals 239,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,iron and steel 241,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,other metals 242,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,metal products except machinery and vehicles 25,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,computers and electronics 26,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,appliances and electrical equipment 27,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,other machinery 28,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,road vehicles 29,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,nonroad vehicles 30,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,other manufacturing 31T33,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,energy pipelines and gas processing 352T353,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,water and waste 36T39,CO2] : test</t>
+  </si>
+  <si>
+    <t>Industrial Sector Energy Related Emissions before CCS[hydrogen if,construction 41T43,CO2] : test</t>
   </si>
 </sst>
 </file>
@@ -2037,7 +2037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -3480,7 +3480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000817FC-5CAD-42B5-92F8-1A675198574D}">
   <dimension ref="A25:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
@@ -3715,8 +3715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D869D793-4D45-441A-BEF3-5973BA28AC13}">
   <dimension ref="A1:AE300"/>
   <sheetViews>
-    <sheetView topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="B283" sqref="B283"/>
+    <sheetView topLeftCell="A265" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:AE280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12349,61 +12349,61 @@
         <v>0</v>
       </c>
       <c r="M94" s="38">
-        <v>943243</v>
+        <v>1001080</v>
       </c>
       <c r="N94" s="38">
-        <v>1871960</v>
+        <v>2002150</v>
       </c>
       <c r="O94" s="38">
-        <v>2836590</v>
+        <v>3003230</v>
       </c>
       <c r="P94" s="38">
-        <v>3769100</v>
+        <v>4004300</v>
       </c>
       <c r="Q94" s="38">
-        <v>4690350</v>
+        <v>5005380</v>
       </c>
       <c r="R94" s="38">
-        <v>4686590</v>
+        <v>5005380</v>
       </c>
       <c r="S94" s="38">
-        <v>4645910</v>
+        <v>5005380</v>
       </c>
       <c r="T94" s="38">
-        <v>4681080</v>
+        <v>5005380</v>
       </c>
       <c r="U94" s="38">
-        <v>4695760</v>
+        <v>5005380</v>
       </c>
       <c r="V94" s="38">
-        <v>4687030</v>
+        <v>5005380</v>
       </c>
       <c r="W94" s="38">
-        <v>4670400</v>
+        <v>5005380</v>
       </c>
       <c r="X94" s="38">
-        <v>4669000</v>
+        <v>5005380</v>
       </c>
       <c r="Y94" s="38">
-        <v>4686670</v>
+        <v>5005380</v>
       </c>
       <c r="Z94" s="38">
-        <v>4701120</v>
+        <v>5005380</v>
       </c>
       <c r="AA94" s="38">
-        <v>4720810</v>
+        <v>5005380</v>
       </c>
       <c r="AB94" s="38">
-        <v>4690790</v>
+        <v>5005380</v>
       </c>
       <c r="AC94" s="38">
-        <v>4679380</v>
+        <v>5005380</v>
       </c>
       <c r="AD94" s="38">
-        <v>4700960</v>
+        <v>5005380</v>
       </c>
       <c r="AE94" s="38">
-        <v>4704050</v>
+        <v>5005380</v>
       </c>
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove IRA from recently edited files
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
+++ b/InputData/ccs/BFoCPAbI/BAU Fraction of CCS Potential Achieved by Industry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\ccs\BFoCPAbI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A36A933-BC91-4634-BA18-BDCAB23ADDCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3796E7-6D09-4296-B1AF-1E2B8ACD4CE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1577,7 +1577,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1637,6 +1637,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3497,7 +3498,7 @@
   <dimension ref="A25:H53"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:E49"/>
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3546,10 +3547,10 @@
         <v>14</v>
       </c>
       <c r="C29">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D29">
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3581,14 +3582,14 @@
       <c r="A35" t="s">
         <v>9</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>60</v>
+      <c r="B35" s="39">
+        <v>0</v>
+      </c>
+      <c r="C35" s="39">
+        <v>0</v>
+      </c>
+      <c r="D35" s="39">
+        <v>28</v>
       </c>
       <c r="E35" t="s">
         <v>162</v>
@@ -3598,14 +3599,14 @@
       <c r="A36" t="s">
         <v>10</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="39">
         <v>2</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="39">
         <v>53</v>
       </c>
-      <c r="D36">
-        <v>53</v>
+      <c r="D36" s="39">
+        <v>66</v>
       </c>
       <c r="E36" t="s">
         <v>156</v>
@@ -3615,38 +3616,44 @@
       <c r="A37" t="s">
         <v>11</v>
       </c>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>50</v>
+      <c r="B39" s="39">
+        <v>0</v>
+      </c>
+      <c r="C39" s="39">
+        <v>0</v>
+      </c>
+      <c r="D39" s="39">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>14</v>
+      <c r="B40" s="39">
+        <v>0</v>
+      </c>
+      <c r="C40" s="39">
+        <v>0</v>
+      </c>
+      <c r="D40" s="39">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3710,11 +3717,11 @@
       </c>
       <c r="C53">
         <f>SUM(C27:C51)</f>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D53">
         <f>SUM(D27:D51)</f>
-        <v>193</v>
+        <v>118</v>
       </c>
       <c r="E53" t="s">
         <v>157</v>
@@ -31685,83 +31692,83 @@
       </c>
       <c r="L10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!L1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!L282</f>
-        <v>6.797194122498923E-2</v>
+        <v>3.1720239238320055E-2</v>
       </c>
       <c r="M10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!M1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!M282</f>
-        <v>0.13719088843809527</v>
+        <v>6.4022414604438208E-2</v>
       </c>
       <c r="N10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!N1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!N282</f>
-        <v>0.21026259730598132</v>
+        <v>9.8122545409453713E-2</v>
       </c>
       <c r="O10">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!O1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!O282</f>
-        <v>0.28255903414752725</v>
+        <v>0.13186088260217724</v>
       </c>
       <c r="P10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!P282</f>
-        <v>0.3573196573135618</v>
+        <v>0.16674917341299553</v>
       </c>
       <c r="Q10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!Q282</f>
-        <v>0.36188854966600742</v>
+        <v>0.16888132317747012</v>
       </c>
       <c r="R10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!R282</f>
-        <v>0.36636970193288443</v>
+        <v>0.17097252756867942</v>
       </c>
       <c r="S10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!S282</f>
-        <v>0.37148422179265589</v>
+        <v>0.17335930350323941</v>
       </c>
       <c r="T10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!T282</f>
-        <v>0.37482682805313933</v>
+        <v>0.17491918642479837</v>
       </c>
       <c r="U10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!U282</f>
-        <v>0.3790537279381066</v>
+        <v>0.17689173970444974</v>
       </c>
       <c r="V10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!V282</f>
-        <v>0.38100597023700644</v>
+        <v>0.17780278611060299</v>
       </c>
       <c r="W10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!W282</f>
-        <v>0.38201956916181673</v>
+        <v>0.17827579894218112</v>
       </c>
       <c r="X10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!X282</f>
-        <v>0.38771762348539407</v>
+        <v>0.18093489095985058</v>
       </c>
       <c r="Y10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!Y282</f>
-        <v>0.39384846353474839</v>
+        <v>0.18379594964954926</v>
       </c>
       <c r="Z10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!Z282</f>
-        <v>0.40101540913707018</v>
+        <v>0.18714052426396607</v>
       </c>
       <c r="AA10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AA282</f>
-        <v>0.41191331250564672</v>
+        <v>0.19222621250263514</v>
       </c>
       <c r="AB10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AB282</f>
-        <v>0.41525074403362489</v>
+        <v>0.19378368054902495</v>
       </c>
       <c r="AC10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AC282</f>
-        <v>0.41011353219867458</v>
+        <v>0.19138631502604814</v>
       </c>
       <c r="AD10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AD282</f>
-        <v>0.411683249786368</v>
+        <v>0.19211884990030506</v>
       </c>
       <c r="AE10" s="38">
         <f>(MAX(TREND('Current and Planned Capacity'!$C$35:$D$35,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-energyEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12)/'BAU Emissions'!AE282</f>
-        <v>0.41796728225246688</v>
+        <v>0.19505139838448454</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -33599,7 +33606,7 @@
       </c>
       <c r="B4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!B$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!B6</f>
-        <v>0.21549849040119179</v>
+        <v>0.21353941321572642</v>
       </c>
       <c r="C4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!C$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!C6</f>
@@ -33607,115 +33614,115 @@
       </c>
       <c r="D4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!D$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!D6</f>
-        <v>0.20477727242789551</v>
+        <v>0.20657356429129811</v>
       </c>
       <c r="E4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!E$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!E6</f>
-        <v>0.20255537970330223</v>
+        <v>0.20604771383611781</v>
       </c>
       <c r="F4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!F$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!F6</f>
-        <v>0.21153343731059926</v>
+        <v>0.21691140605578396</v>
       </c>
       <c r="G4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!G$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!G6</f>
-        <v>0.21409874458437661</v>
+        <v>0.22123536940385582</v>
       </c>
       <c r="H4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!H$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!H6</f>
-        <v>0.21328152881135307</v>
+        <v>0.22202257507411344</v>
       </c>
       <c r="I4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!I$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!I6</f>
-        <v>0.2123795236092286</v>
+        <v>0.22265595217096545</v>
       </c>
       <c r="J4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!J$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!J6</f>
-        <v>0.20976246638696389</v>
+        <v>0.22141593674179522</v>
       </c>
       <c r="K4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!K$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!K6</f>
-        <v>0.21080823195717815</v>
+        <v>0.22398374645450181</v>
       </c>
       <c r="L4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!L$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!L6</f>
-        <v>0.21184826952733757</v>
+        <v>0.22651468818692247</v>
       </c>
       <c r="M4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!M$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!M6</f>
-        <v>0.2148995110638012</v>
+        <v>0.23117977705348311</v>
       </c>
       <c r="N4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!N$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!N6</f>
-        <v>0.21757159751446298</v>
+        <v>0.23543195253430696</v>
       </c>
       <c r="O4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!O$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!O6</f>
-        <v>0.21760789548266654</v>
+        <v>0.23680859214290184</v>
       </c>
       <c r="P4" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$B$29:$C$29,'Current and Planned Capacity'!$B$26:$C$26,'BFoCPAbI-processEmis'!P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!P6</f>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="Q4" s="38">
         <f>P4</f>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="R4" s="38">
         <f t="shared" ref="R4:AE4" si="0">Q4</f>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="S4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="T4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="U4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="V4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="W4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="X4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="Y4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="Z4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="AA4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="AB4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="AC4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="AD4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
       <c r="AE4" s="38">
         <f t="shared" si="0"/>
-        <v>0.21896791807299862</v>
+        <v>0.2395953306450927</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -34334,83 +34341,83 @@
       </c>
       <c r="L11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!L$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!L13</f>
-        <v>0.22394546986301439</v>
+        <v>0.23493147404497516</v>
       </c>
       <c r="M11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!M$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!M13</f>
-        <v>0.2193794882584105</v>
+        <v>0.24090351352149911</v>
       </c>
       <c r="N11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!N$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!N13</f>
-        <v>0.21529611016146474</v>
+        <v>0.24698119807202071</v>
       </c>
       <c r="O11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!O$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!O13</f>
-        <v>0.2115552541092765</v>
+        <v>0.25306798321751411</v>
       </c>
       <c r="P11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!P13</f>
-        <v>0.20710444974798017</v>
+        <v>0.25790365440314517</v>
       </c>
       <c r="Q11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Q13</f>
-        <v>0.20328266288971342</v>
+        <v>0.25314444812681297</v>
       </c>
       <c r="R11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!R13</f>
-        <v>0.2009866814669799</v>
+        <v>0.25028530144944672</v>
       </c>
       <c r="S11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!S13</f>
-        <v>0.19823108000727838</v>
+        <v>0.24685379774491273</v>
       </c>
       <c r="T11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!T13</f>
-        <v>0.19571545716454641</v>
+        <v>0.24372113533698236</v>
       </c>
       <c r="U11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!U13</f>
-        <v>0.1934244735522524</v>
+        <v>0.24086821234808792</v>
       </c>
       <c r="V11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!V13</f>
-        <v>0.1888454451987705</v>
+        <v>0.23516602609658219</v>
       </c>
       <c r="W11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!W13</f>
-        <v>0.18484672023051849</v>
+        <v>0.23018648179649473</v>
       </c>
       <c r="X11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!X13</f>
-        <v>0.18201075560070329</v>
+        <v>0.22665490320087581</v>
       </c>
       <c r="Y11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Y13</f>
-        <v>0.17912169598799371</v>
+        <v>0.22305720632467144</v>
       </c>
       <c r="Z11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Z13</f>
-        <v>0.17774542479331068</v>
+        <v>0.2213433591765756</v>
       </c>
       <c r="AA11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AA13</f>
-        <v>0.1763229194881813</v>
+        <v>0.21957193747584844</v>
       </c>
       <c r="AB11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AB13</f>
-        <v>0.17479083518586616</v>
+        <v>0.21766405891070129</v>
       </c>
       <c r="AC11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AC13</f>
-        <v>0.17257416663073022</v>
+        <v>0.21490367920053202</v>
       </c>
       <c r="AD11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AD13</f>
-        <v>0.16997477617082576</v>
+        <v>0.2116667024014057</v>
       </c>
       <c r="AE11" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$36:$D$36,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AE13</f>
-        <v>0.16781695347732598</v>
+        <v>0.20897960244346259</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -34649,83 +34656,83 @@
       </c>
       <c r="L14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!L$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!L16</f>
-        <v>0.11489402393305781</v>
+        <v>3.4468207179917339E-2</v>
       </c>
       <c r="M14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!M$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!M16</f>
-        <v>0.22736418644182138</v>
+        <v>6.8209255932546412E-2</v>
       </c>
       <c r="N14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!N$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!N16</f>
-        <v>0.33835844722611369</v>
+        <v>0.10150753416783409</v>
       </c>
       <c r="O14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!O$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!O16</f>
-        <v>0.44951843143325088</v>
+        <v>0.13485552942997525</v>
       </c>
       <c r="P14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!P16</f>
-        <v>0.55773370421886859</v>
+        <v>0.16732011126566063</v>
       </c>
       <c r="Q14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Q16</f>
-        <v>0.5488273568737414</v>
+        <v>0.16464820706212246</v>
       </c>
       <c r="R14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!R16</f>
-        <v>0.54194486829114297</v>
+        <v>0.16258346048734293</v>
       </c>
       <c r="S14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!S16</f>
-        <v>0.53668067984960843</v>
+        <v>0.16100420395488257</v>
       </c>
       <c r="T14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!T16</f>
-        <v>0.53100048287309798</v>
+        <v>0.15930014486192945</v>
       </c>
       <c r="U14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!U16</f>
-        <v>0.52683451650173396</v>
+        <v>0.15805035495052022</v>
       </c>
       <c r="V14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!V16</f>
-        <v>0.52135976698720321</v>
+        <v>0.156407930096161</v>
       </c>
       <c r="W14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!W16</f>
-        <v>0.51471980769066816</v>
+        <v>0.15441594230720046</v>
       </c>
       <c r="X14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!X16</f>
-        <v>0.50961167182917289</v>
+        <v>0.15288350154875188</v>
       </c>
       <c r="Y14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Y16</f>
-        <v>0.50724276225646314</v>
+        <v>0.15217282867693899</v>
       </c>
       <c r="Z14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Z16</f>
-        <v>0.50193467907277667</v>
+        <v>0.15058040372183301</v>
       </c>
       <c r="AA14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AA16</f>
-        <v>0.49622828208468234</v>
+        <v>0.14886848462540472</v>
       </c>
       <c r="AB14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AB16</f>
-        <v>0.49170034574933713</v>
+        <v>0.14751010372480117</v>
       </c>
       <c r="AC14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AC16</f>
-        <v>0.48709116942493758</v>
+        <v>0.14612735082748129</v>
       </c>
       <c r="AD14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AD16</f>
-        <v>0.48331568699112676</v>
+        <v>0.14499470609733806</v>
       </c>
       <c r="AE14" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$39:$D$39,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AE16</f>
-        <v>0.47954559099284394</v>
+        <v>0.14386367729785321</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -34774,83 +34781,83 @@
       </c>
       <c r="L15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!L$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!L17</f>
-        <v>5.6976723141277615E-2</v>
+        <v>0</v>
       </c>
       <c r="M15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!M$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!M17</f>
-        <v>0.11421969265239283</v>
+        <v>0</v>
       </c>
       <c r="N15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!N$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!N17</f>
-        <v>0.16935113783565861</v>
+        <v>0</v>
       </c>
       <c r="O15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!O$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!O17</f>
-        <v>0.22627182807326129</v>
+        <v>0</v>
       </c>
       <c r="P15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!P17</f>
-        <v>0.28160154640108814</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Q17</f>
-        <v>0.27973236699032333</v>
+        <v>0</v>
       </c>
       <c r="R15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!R17</f>
-        <v>0.27941259976696908</v>
+        <v>0</v>
       </c>
       <c r="S15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!S17</f>
-        <v>0.27669248616271735</v>
+        <v>0</v>
       </c>
       <c r="T15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!T17</f>
-        <v>0.27427080596515319</v>
+        <v>0</v>
       </c>
       <c r="U15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!U17</f>
-        <v>0.27457890617405589</v>
+        <v>0</v>
       </c>
       <c r="V15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!V17</f>
-        <v>0.27274061847371628</v>
+        <v>0</v>
       </c>
       <c r="W15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!W17</f>
-        <v>0.26860455195180716</v>
+        <v>0</v>
       </c>
       <c r="X15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!X17</f>
-        <v>0.26655413552469415</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Y17</f>
-        <v>0.26620577464184769</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!Z17</f>
-        <v>0.26754612771031583</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AA17</f>
-        <v>0.26937419250181238</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AB17</f>
-        <v>0.2701482562733693</v>
+        <v>0</v>
       </c>
       <c r="AC15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AC17</f>
-        <v>0.26990960940386982</v>
+        <v>0</v>
       </c>
       <c r="AD15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AD17</f>
-        <v>0.26813310912258065</v>
+        <v>0</v>
       </c>
       <c r="AE15" s="38">
         <f>MAX(TREND('Current and Planned Capacity'!$C$40:$D$40,'Current and Planned Capacity'!$C$26:$D$26,'BFoCPAbI-processEmis'!$P$1),0)*'Capacity Factor Data'!$A$45*10^12/'BAU Emissions'!AE17</f>
-        <v>0.26719517083094069</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>